<commit_message>
updating code to include fluoro and eto
</commit_message>
<xml_diff>
--- a/ETO_Fluoro_Use.xlsx
+++ b/ETO_Fluoro_Use.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10608"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D563AD-571B-CB41-8CED-7DFFA43D3CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E377051-A351-1543-99E2-DA87614BF91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33760" yWindow="3760" windowWidth="25020" windowHeight="15620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2140" yWindow="1180" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ETO Use" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="102">
   <si>
     <t>Date</t>
   </si>
@@ -295,13 +295,55 @@
   </si>
   <si>
     <t>CL015, CL006, CL007</t>
+  </si>
+  <si>
+    <t> 01-01777-2000-30203-64300</t>
+  </si>
+  <si>
+    <t>01-01777-5000-51006420-64300</t>
+  </si>
+  <si>
+    <t>01-01777-5000-51006798-64300</t>
+  </si>
+  <si>
+    <t>01-00879-6000-29784-64300</t>
+  </si>
+  <si>
+    <t>01-00879-2000-28647-64300</t>
+  </si>
+  <si>
+    <t>01-00879-5000-59007835-64300</t>
+  </si>
+  <si>
+    <t>01-00879-5000-59700310-64300</t>
+  </si>
+  <si>
+    <t>01-00879-5000-59318460-64300</t>
+  </si>
+  <si>
+    <t>01-01755-5000-51006844-64300</t>
+  </si>
+  <si>
+    <t>01-00213-5000-51004696-64300</t>
+  </si>
+  <si>
+    <t>01-01777-2000-30203-64300</t>
+  </si>
+  <si>
+    <t>01-00213-5000-55900809-64300</t>
+  </si>
+  <si>
+    <t>01-01777-2000-30670-64300</t>
+  </si>
+  <si>
+    <t>Chartfield</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,13 +357,60 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF242424"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -336,10 +425,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1774,7 +1890,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10:XFD10"/>
@@ -1782,329 +1898,377 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="21.5" customWidth="1"/>
-    <col min="5" max="5" width="136" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="136" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>42</v>
       </c>
       <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>50</v>
       </c>
       <c r="D2" t="s">
         <v>50</v>
       </c>
       <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>53</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>53</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>35</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>2148</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>46</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>53</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>53</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>37</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>2140</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" t="s">
         <v>31</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>54</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>54</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" t="s">
         <v>33</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>54</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>54</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>44</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>55</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" t="s">
         <v>30</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>17</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>53</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>41</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>2200</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>57</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" t="s">
         <v>59</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>5</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>53</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>60</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>1848</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>58</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" t="s">
         <v>59</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>5</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>53</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>61</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>2057</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>56</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" t="s">
         <v>27</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>53</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>62</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>2336</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>76</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" t="s">
         <v>59</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>5</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>53</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>2348</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>79</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" t="s">
         <v>81</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>82</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2116,10 +2280,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2498,13 +2662,36 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="1"/>
+      <c r="A47" s="1">
+        <v>45840</v>
+      </c>
+      <c r="B47" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="1"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1"/>
+      <c r="A48" s="1">
+        <v>45846</v>
+      </c>
+      <c r="B48" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>45852</v>
+      </c>
+      <c r="B49" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>45861</v>
+      </c>
+      <c r="B50" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2517,7 +2704,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2531,16 +2718,36 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1">
+        <v>45855</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1">
+        <v>45860</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1">
+        <v>45866</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1">
+        <v>45867</v>
+      </c>
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>

</xml_diff>

<commit_message>
updating with august charges
</commit_message>
<xml_diff>
--- a/ETO_Fluoro_Use.xlsx
+++ b/ETO_Fluoro_Use.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10824"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E377051-A351-1543-99E2-DA87614BF91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A383358E-A2C6-104D-A5DE-D57013A73647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="1180" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ETO Use" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="102">
   <si>
     <t>Date</t>
   </si>
@@ -2280,10 +2280,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2693,6 +2693,38 @@
         <v>79</v>
       </c>
     </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>45874</v>
+      </c>
+      <c r="B51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>45876</v>
+      </c>
+      <c r="B52" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>45883</v>
+      </c>
+      <c r="B53" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>45890</v>
+      </c>
+      <c r="B54" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2701,10 +2733,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D46EC14E-6917-0943-8C04-E0E228EF2377}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2750,9 +2782,39 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1">
+        <v>45881</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>45887</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>45888</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>45894</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated code to include codes only in fluoro
</commit_message>
<xml_diff>
--- a/ETO_Fluoro_Use.xlsx
+++ b/ETO_Fluoro_Use.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11003"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A383358E-A2C6-104D-A5DE-D57013A73647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29012DD0-B129-5749-8846-02B02B89F382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ETO Use" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="104">
   <si>
     <t>Date</t>
   </si>
@@ -337,6 +337,12 @@
   </si>
   <si>
     <t>Chartfield</t>
+  </si>
+  <si>
+    <t>CL016</t>
+  </si>
+  <si>
+    <t>01-01777-5000-54903702-64303</t>
   </si>
 </sst>
 </file>
@@ -1890,15 +1896,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="21.5" customWidth="1"/>
     <col min="6" max="6" width="136" bestFit="1" customWidth="1"/>
@@ -2272,7 +2278,25 @@
         <v>53</v>
       </c>
     </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2280,10 +2304,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2725,6 +2749,46 @@
         <v>79</v>
       </c>
     </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>45911</v>
+      </c>
+      <c r="B55" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>45924</v>
+      </c>
+      <c r="B56" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>45929</v>
+      </c>
+      <c r="B57" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>45937</v>
+      </c>
+      <c r="B58" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>45952</v>
+      </c>
+      <c r="B59" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2733,10 +2797,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D46EC14E-6917-0943-8C04-E0E228EF2377}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2813,6 +2877,70 @@
         <v>76</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>45915</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>45917</v>
+      </c>
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>45918</v>
+      </c>
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>45922</v>
+      </c>
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>45944</v>
+      </c>
+      <c r="B14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>45945</v>
+      </c>
+      <c r="B15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>45958</v>
+      </c>
+      <c r="B16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>45959</v>
+      </c>
+      <c r="B17" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>